<commit_message>
refactored spreadsheet generator into base class and derived classes
</commit_message>
<xml_diff>
--- a/SpreadsheetUtility/SpreadsheetUtility.UI.Console/output.xlsx
+++ b/SpreadsheetUtility/SpreadsheetUtility.UI.Console/output.xlsx
@@ -1,21 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <x:workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\Utilities\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5F42B8-BA34-4018-9F88-5577A4BA2861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Service Mapping" sheetId="1" r:id="rId2"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Service Mapping" sheetId="2" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="162913"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </x:ext>
+  </x:extLst>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
+    <x:t>Id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CarModel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LicensePlate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ManufacturingYear</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Features</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CarModelA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LicensePlate1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AirConditioning
+PowerSteering</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CarModelB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LicensePlate2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PowerSteering
+BucketSeats</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CarModelC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LicensePlate3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AirConditioning
+BucketSeats</x:t>
+  </x:si>
+  <x:si>
     <x:t>keyColumn</x:t>
   </x:si>
   <x:si>
@@ -28,26 +86,24 @@
     <x:t>PowerSteering</x:t>
   </x:si>
   <x:si>
-    <x:t>CarModelA</x:t>
-  </x:si>
-  <x:si>
     <x:t>X</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CarModelB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CarModelC</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -65,38 +121,35 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <x:alignment wrapText="1"/>
     </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -111,44 +164,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -175,14 +228,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -209,6 +263,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -220,170 +275,243 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E4"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="J9" sqref="J9"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:cols>
+    <x:col min="1" max="1" width="2.664062" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="10.554688" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="12.886719" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="17.441406" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="5" max="5" width="14.664062" style="0" bestFit="1" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A2" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D2" s="1">
+        <x:v>1985</x:v>
+      </x:c>
+      <x:c r="E2" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A3" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D3" s="1">
+        <x:v>1995</x:v>
+      </x:c>
+      <x:c r="E3" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A4" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D4" s="0">
+        <x:v>1992</x:v>
+      </x:c>
+      <x:c r="E4" s="1" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="9" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -396,49 +524,49 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="A3" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="A4" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>